<commit_message>
Actualización de archivos JSON y scripts 29 de agosto
</commit_message>
<xml_diff>
--- a/Segumiento_proteccion.xlsx
+++ b/Segumiento_proteccion.xlsx
@@ -418,7 +418,7 @@
 </t>
   </si>
   <si>
-    <t>PRUEBAS PROTECCION</t>
+    <t>PRUEBAS CIONPRO</t>
   </si>
   <si>
     <t>Alejandro Cardona Ocampo</t>
@@ -3944,7 +3944,7 @@
       <c r="L20" s="82"/>
       <c r="M20" s="24">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N20" s="56"/>
       <c r="O20" s="57"/>
@@ -3979,7 +3979,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="39">
         <f>IF(ISBLANK(L21), NETWORKDAYS(I20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(I20, L21, Hoja2!$A$1:$A$18))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N21" s="72"/>
       <c r="O21" s="60"/>
@@ -4071,7 +4071,7 @@
       <c r="L23" s="85"/>
       <c r="M23" s="39">
         <f>IF(ISBLANK(L23), NETWORKDAYS(J23, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J23, L23, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N23" s="72"/>
       <c r="O23" s="60"/>
@@ -4257,7 +4257,7 @@
       <c r="L27" s="85"/>
       <c r="M27" s="39">
         <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32769</v>
       </c>
       <c r="N27" s="72"/>
       <c r="O27" s="60"/>
@@ -41329,7 +41329,7 @@
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="F2:F29 F41:F940">
-      <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS PROTECCION,PRUEBAS IMAGINE"</formula1>
+      <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CIONPRO,PRUEBAS IMAGINE"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 11 de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_proteccion.xlsx
+++ b/Segumiento_proteccion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="239">
   <si>
     <t>Asignado a</t>
   </si>
@@ -425,6 +425,18 @@
   </si>
   <si>
     <t>Desacople de agente de clasificación y su lógica y acople del mismo dento del sistema distribuido. Adicionalmente, acople de la plataforma de agentes y todas las otras aplicaciones del sistema</t>
+  </si>
+  <si>
+    <t>Interno-H10</t>
+  </si>
+  <si>
+    <t>Generación de ambiente local a través de lo generado en el ambiente de pruebas, para facilitar la construcción de otros servicios</t>
+  </si>
+  <si>
+    <t>Interno-H11</t>
+  </si>
+  <si>
+    <t>Generación de servicio para el tratamiento de datos usando agentes</t>
   </si>
   <si>
     <t>Alejandro Cardona Ocampo</t>
@@ -3950,7 +3962,7 @@
       <c r="L20" s="82"/>
       <c r="M20" s="24">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="N20" s="56"/>
       <c r="O20" s="57"/>
@@ -3985,7 +3997,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="39">
         <f>IF(ISBLANK(L21), NETWORKDAYS(I20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(I20, L21, Hoja2!$A$1:$A$18))</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="N21" s="72"/>
       <c r="O21" s="60"/>
@@ -4077,7 +4089,7 @@
       <c r="L23" s="85"/>
       <c r="M23" s="39">
         <f>IF(ISBLANK(L23), NETWORKDAYS(J23, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J23, L23, Hoja2!$A$1:$A$18))</f>
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="N23" s="72"/>
       <c r="O23" s="60"/>
@@ -4263,7 +4275,7 @@
       <c r="L27" s="85"/>
       <c r="M27" s="39">
         <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
-        <v>32772</v>
+        <v>32778</v>
       </c>
       <c r="N27" s="72"/>
       <c r="O27" s="60"/>
@@ -4461,14 +4473,90 @@
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="97"/>
-      <c r="G32" s="98"/>
-      <c r="Q32" s="99"/>
+      <c r="A32" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="77">
+        <v>100.0</v>
+      </c>
+      <c r="H32" s="65">
+        <v>2.0</v>
+      </c>
+      <c r="I32" s="66">
+        <v>45904.0</v>
+      </c>
+      <c r="J32" s="66">
+        <v>45908.0</v>
+      </c>
+      <c r="K32" s="67">
+        <v>45909.0</v>
+      </c>
+      <c r="L32" s="67">
+        <v>45908.0</v>
+      </c>
+      <c r="M32" s="24">
+        <f>IF(ISBLANK(L32), NETWORKDAYS(J32, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J32, L32, Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N32" s="67"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
-      <c r="B33" s="100"/>
-      <c r="G33" s="101"/>
-      <c r="Q33" s="102"/>
+      <c r="A33" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="90">
+        <v>50.0</v>
+      </c>
+      <c r="H33" s="48">
+        <v>4.0</v>
+      </c>
+      <c r="I33" s="54">
+        <v>45904.0</v>
+      </c>
+      <c r="J33" s="54">
+        <v>45909.0</v>
+      </c>
+      <c r="K33" s="71">
+        <v>45912.0</v>
+      </c>
+      <c r="L33" s="71"/>
+      <c r="M33" s="39">
+        <f>IF(ISBLANK(L33), NETWORKDAYS(J33, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J33, L33, Hoja2!$A$1:$A$18))</f>
+        <v>3</v>
+      </c>
+      <c r="N33" s="71"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="96"/>
+      <c r="Q33" s="43" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="97"/>
@@ -41413,10 +41501,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L20 I21 K21:L21 I22:L31 N2:O31 I41:L940 N41:O940">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L20 I21 K21:L21 I22:L33 N2:O33 I41:L940 N41:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F31 F41:F940">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F33 F41:F940">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -41514,19 +41602,19 @@
     </row>
     <row r="2" ht="29.25" customHeight="1">
       <c r="A2" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B2" s="144" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="145" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D2" s="144" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="144" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F2" s="146" t="s">
         <v>21</v>
@@ -41561,19 +41649,19 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B3" s="144" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="145" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D3" s="144" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F3" s="146" t="s">
         <v>21</v>
@@ -41608,19 +41696,19 @@
     </row>
     <row r="4" ht="39.0" customHeight="1">
       <c r="A4" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B4" s="144" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="145" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D4" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="144" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F4" s="146" t="s">
         <v>21</v>
@@ -41659,19 +41747,19 @@
     </row>
     <row r="5">
       <c r="A5" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B5" s="144" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D5" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="160" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F5" s="146" t="s">
         <v>21</v>
@@ -41710,19 +41798,19 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B6" s="144" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="145" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D6" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="162" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F6" s="163" t="s">
         <v>21</v>
@@ -41761,19 +41849,19 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B7" s="144" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="145" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D7" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="144" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F7" s="165" t="s">
         <v>21</v>
@@ -41812,19 +41900,19 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B8" s="144" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="145" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D8" s="144" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="167" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F8" s="146" t="s">
         <v>21</v>
@@ -41859,17 +41947,17 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B9" s="144" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="171" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D9" s="172"/>
       <c r="E9" s="144" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F9" s="165" t="s">
         <v>21</v>
@@ -41906,17 +41994,17 @@
     </row>
     <row r="10" ht="93.0" customHeight="1">
       <c r="A10" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" s="144" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="171" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D10" s="172"/>
       <c r="E10" s="144" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F10" s="165" t="s">
         <v>21</v>
@@ -41951,19 +42039,19 @@
     </row>
     <row r="11">
       <c r="A11" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B11" s="144" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="145" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D11" s="144" t="s">
         <v>41</v>
       </c>
       <c r="E11" s="174" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F11" s="165" t="s">
         <v>21</v>
@@ -42000,19 +42088,19 @@
     </row>
     <row r="12" ht="29.25" customHeight="1">
       <c r="A12" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B12" s="144" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="175" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D12" s="144" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="144" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F12" s="165" t="s">
         <v>21</v>
@@ -42049,19 +42137,19 @@
     </row>
     <row r="13" ht="29.25" customHeight="1">
       <c r="A13" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B13" s="144" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="171" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D13" s="144" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="144" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F13" s="165" t="s">
         <v>21</v>
@@ -42096,7 +42184,7 @@
     </row>
     <row r="14" ht="29.25" customHeight="1">
       <c r="A14" s="143" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B14" s="144" t="s">
         <v>60</v>
@@ -42106,7 +42194,7 @@
       </c>
       <c r="D14" s="176"/>
       <c r="E14" s="162" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F14" s="170" t="s">
         <v>21</v>
@@ -42184,7 +42272,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="177" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B1" s="177" t="s">
         <v>2</v>
@@ -42211,13 +42299,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="180" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="K1" s="177" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="L1" s="181" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M1" s="182"/>
       <c r="N1" s="182"/>
@@ -42236,14 +42324,14 @@
     </row>
     <row r="2">
       <c r="A2" s="183" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B2" s="184" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C2" s="185"/>
       <c r="D2" s="186" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E2" s="187">
         <v>45526.0</v>
@@ -42257,7 +42345,7 @@
       <c r="J2" s="185"/>
       <c r="K2" s="185"/>
       <c r="L2" s="185" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="M2" s="188"/>
       <c r="N2" s="188"/>
@@ -42276,13 +42364,13 @@
     </row>
     <row r="3">
       <c r="A3" s="189" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B3" s="190" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C3" s="191" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D3" s="191" t="s">
         <v>21</v>
@@ -42306,7 +42394,7 @@
       </c>
       <c r="K3" s="193"/>
       <c r="L3" s="195" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M3" s="182"/>
       <c r="N3" s="182"/>
@@ -42325,16 +42413,16 @@
     </row>
     <row r="4">
       <c r="A4" s="196" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B4" s="197" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C4" s="196" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D4" s="198" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E4" s="199">
         <v>45581.0</v>
@@ -42357,7 +42445,7 @@
       </c>
       <c r="K4" s="199"/>
       <c r="L4" s="196" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="M4" s="202"/>
       <c r="N4" s="202"/>
@@ -42376,13 +42464,13 @@
     </row>
     <row r="5">
       <c r="A5" s="181" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B5" s="197" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C5" s="191" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D5" s="203" t="s">
         <v>65</v>
@@ -42406,7 +42494,7 @@
       </c>
       <c r="K5" s="192"/>
       <c r="L5" s="195" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="M5" s="182"/>
       <c r="N5" s="182"/>
@@ -42425,16 +42513,16 @@
     </row>
     <row r="6">
       <c r="A6" s="204" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B6" s="204" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C6" s="198" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D6" s="204" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E6" s="205">
         <v>45602.0</v>
@@ -42455,7 +42543,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="206" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="M6" s="207"/>
       <c r="N6" s="208"/>
@@ -42474,13 +42562,13 @@
     </row>
     <row r="7">
       <c r="A7" s="181" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B7" s="190" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C7" s="209" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D7" s="203" t="s">
         <v>65</v>
@@ -42504,7 +42592,7 @@
       </c>
       <c r="K7" s="203"/>
       <c r="L7" s="211" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="M7" s="212"/>
       <c r="N7" s="212"/>
@@ -42523,14 +42611,14 @@
     </row>
     <row r="8">
       <c r="A8" s="213" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B8" s="214" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C8" s="215"/>
       <c r="D8" s="215" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E8" s="216">
         <v>45603.0</v>
@@ -42551,7 +42639,7 @@
       </c>
       <c r="K8" s="216"/>
       <c r="L8" s="218" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="M8" s="182"/>
       <c r="N8" s="182"/>
@@ -42570,16 +42658,16 @@
     </row>
     <row r="9">
       <c r="A9" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B9" s="220" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C9" s="221" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D9" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E9" s="223">
         <v>45671.0</v>
@@ -42588,7 +42676,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="221" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H9" s="223">
         <v>45680.0</v>
@@ -42602,7 +42690,7 @@
       </c>
       <c r="K9" s="221"/>
       <c r="L9" s="225" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M9" s="226"/>
       <c r="N9" s="226"/>
@@ -42621,14 +42709,14 @@
     </row>
     <row r="10">
       <c r="A10" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B10" s="227"/>
       <c r="C10" s="225" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D10" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E10" s="223">
         <v>45671.0</v>
@@ -42647,7 +42735,7 @@
       <c r="J10" s="221"/>
       <c r="K10" s="221"/>
       <c r="L10" s="225" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M10" s="226"/>
       <c r="N10" s="226"/>
@@ -42666,14 +42754,14 @@
     </row>
     <row r="11">
       <c r="A11" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B11" s="227"/>
       <c r="C11" s="225" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D11" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E11" s="223">
         <v>45671.0</v>
@@ -42692,7 +42780,7 @@
       <c r="J11" s="221"/>
       <c r="K11" s="221"/>
       <c r="L11" s="225" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M11" s="226"/>
       <c r="N11" s="226"/>
@@ -42711,14 +42799,14 @@
     </row>
     <row r="12">
       <c r="A12" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B12" s="227"/>
       <c r="C12" s="225" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D12" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E12" s="223">
         <v>45671.0</v>
@@ -42737,7 +42825,7 @@
       <c r="J12" s="221"/>
       <c r="K12" s="221"/>
       <c r="L12" s="225" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M12" s="226"/>
       <c r="N12" s="226"/>
@@ -42756,14 +42844,14 @@
     </row>
     <row r="13">
       <c r="A13" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B13" s="227"/>
       <c r="C13" s="225" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D13" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E13" s="223">
         <v>45671.0</v>
@@ -42782,7 +42870,7 @@
       <c r="J13" s="221"/>
       <c r="K13" s="221"/>
       <c r="L13" s="225" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M13" s="226"/>
       <c r="N13" s="226"/>
@@ -42801,14 +42889,14 @@
     </row>
     <row r="14">
       <c r="A14" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B14" s="227"/>
       <c r="C14" s="225" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D14" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E14" s="223">
         <v>45671.0</v>
@@ -42827,7 +42915,7 @@
       <c r="J14" s="221"/>
       <c r="K14" s="221"/>
       <c r="L14" s="221" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="M14" s="226"/>
       <c r="N14" s="226"/>
@@ -42846,14 +42934,14 @@
     </row>
     <row r="15">
       <c r="A15" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B15" s="227"/>
       <c r="C15" s="225" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D15" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E15" s="223">
         <v>45671.0</v>
@@ -42872,7 +42960,7 @@
       <c r="J15" s="221"/>
       <c r="K15" s="221"/>
       <c r="L15" s="221" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="M15" s="226"/>
       <c r="N15" s="226"/>
@@ -42891,14 +42979,14 @@
     </row>
     <row r="16">
       <c r="A16" s="219" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B16" s="228"/>
       <c r="C16" s="229" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D16" s="222" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E16" s="223">
         <v>45681.0</v>
@@ -42917,7 +43005,7 @@
       <c r="J16" s="221"/>
       <c r="K16" s="221"/>
       <c r="L16" s="225" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M16" s="226"/>
       <c r="N16" s="226"/>
@@ -49453,7 +49541,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="226" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49461,7 +49549,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="226" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49469,7 +49557,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="226" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49477,7 +49565,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="226" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49485,7 +49573,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="226" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49493,7 +49581,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="226" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49501,7 +49589,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="226" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49509,7 +49597,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="226" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49517,7 +49605,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="226" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49525,7 +49613,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="226" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49533,7 +49621,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="226" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49541,7 +49629,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="226" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49549,7 +49637,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="226" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49557,7 +49645,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="226" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49565,7 +49653,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="226" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49573,7 +49661,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="226" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49581,7 +49669,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="226" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49589,7 +49677,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="226" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50605,7 +50693,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="231" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B1" s="226"/>
       <c r="C1" s="226"/>
@@ -50663,7 +50751,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="232" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B3" s="233">
         <v>45596.0</v>
@@ -50956,261 +51044,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="236" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B4" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C4" s="238" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O4" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P4" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U4" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="V4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE4" s="241" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF4" s="239" t="s">
         <v>205</v>
       </c>
-      <c r="AF4" s="239" t="s">
-        <v>201</v>
-      </c>
       <c r="AG4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL4" s="241" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="AM4" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AN4" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AO4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP4" s="241" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="AQ4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS4" s="241" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="AT4" s="242" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AV4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY4" s="241" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="AZ4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BA4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BH4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI4" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ4" s="241" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="BK4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BL4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BM4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BN4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BO4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BP4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BQ4" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BR4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CA4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CB4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CC4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CD4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG4" s="239"/>
       <c r="CH4" s="239"/>
       <c r="CI4" s="241" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="CJ4" s="239"/>
       <c r="CK4" s="239"/>
@@ -51222,249 +51310,249 @@
       <c r="CQ4" s="239"/>
       <c r="CR4" s="239"/>
       <c r="CS4" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="236" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B5" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="M5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="N5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="O5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="P5" s="240" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="Q5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U5" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="V5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE5" s="243"/>
       <c r="AF5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL5" s="243"/>
       <c r="AM5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AN5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AO5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP5" s="243"/>
       <c r="AQ5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AR5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AS5" s="243"/>
       <c r="AT5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AU5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AV5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AW5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AX5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AY5" s="243"/>
       <c r="AZ5" s="239" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BA5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BH5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI5" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ5" s="243"/>
       <c r="BK5" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL5" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN5" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BP5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BQ5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BR5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CA5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CB5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CC5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CD5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG5" s="239"/>
       <c r="CH5" s="239"/>
@@ -51479,249 +51567,249 @@
       <c r="CQ5" s="239"/>
       <c r="CR5" s="239"/>
       <c r="CS5" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="236" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B6" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K6" s="244" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="L6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O6" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P6" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U6" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="V6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE6" s="243"/>
       <c r="AF6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL6" s="243"/>
       <c r="AM6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AN6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AO6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP6" s="243"/>
       <c r="AQ6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS6" s="243"/>
       <c r="AT6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AV6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY6" s="243"/>
       <c r="AZ6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BA6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BH6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI6" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ6" s="243"/>
       <c r="BK6" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL6" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM6" s="239" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="BN6" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BP6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BQ6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BR6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CA6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CB6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CC6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CD6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG6" s="239"/>
       <c r="CH6" s="239"/>
@@ -51736,198 +51824,198 @@
       <c r="CQ6" s="239"/>
       <c r="CR6" s="239"/>
       <c r="CS6" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="236" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B7" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L7" s="244" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="M7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O7" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P7" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U7" s="240" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="V7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z7" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AA7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE7" s="243"/>
       <c r="AF7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL7" s="243"/>
       <c r="AM7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AN7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AO7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP7" s="243"/>
       <c r="AQ7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS7" s="243"/>
       <c r="AT7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU7" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AV7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY7" s="243"/>
       <c r="AZ7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BA7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BH7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI7" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ7" s="243"/>
       <c r="BK7" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL7" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN7" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO7" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BP7" s="239"/>
       <c r="BQ7" s="239"/>
@@ -51935,16 +52023,16 @@
       <c r="BS7" s="239"/>
       <c r="BT7" s="239"/>
       <c r="BU7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX7" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY7" s="239"/>
       <c r="BZ7" s="239"/>
@@ -51970,220 +52058,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="236" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B8" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L8" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="M8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O8" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P8" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U8" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="V8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W8" s="239" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="X8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB8" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AC8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE8" s="243"/>
       <c r="AF8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL8" s="243"/>
       <c r="AM8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AN8" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AO8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP8" s="243"/>
       <c r="AQ8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS8" s="243"/>
       <c r="AT8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AV8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY8" s="243"/>
       <c r="AZ8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BA8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG8" s="239" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="BH8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI8" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ8" s="243"/>
       <c r="BK8" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL8" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN8" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BP8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BQ8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BR8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW8" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX8" s="239" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="BY8" s="239"/>
       <c r="BZ8" s="239"/>
@@ -52209,244 +52297,244 @@
     </row>
     <row r="9">
       <c r="A9" s="236" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B9" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="L9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O9" s="244" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="P9" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U9" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="V9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE9" s="243"/>
       <c r="AF9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL9" s="243"/>
       <c r="AM9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AN9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AO9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP9" s="243"/>
       <c r="AQ9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS9" s="243"/>
       <c r="AT9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AV9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY9" s="243"/>
       <c r="AZ9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BA9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BH9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI9" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ9" s="243"/>
       <c r="BK9" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL9" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN9" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BP9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BQ9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BR9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CA9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CB9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CC9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CD9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG9" s="239"/>
       <c r="CH9" s="239"/>
@@ -52461,249 +52549,249 @@
       <c r="CQ9" s="239"/>
       <c r="CR9" s="239"/>
       <c r="CS9" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="236" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B10" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="L10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="O10" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P10" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Q10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="R10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U10" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="V10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AE10" s="243"/>
       <c r="AF10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AL10" s="243"/>
       <c r="AM10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AN10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AO10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP10" s="243"/>
       <c r="AQ10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS10" s="243"/>
       <c r="AT10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AV10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY10" s="243"/>
       <c r="AZ10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BA10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BB10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BC10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BD10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BE10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BF10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BG10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BH10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI10" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ10" s="243"/>
       <c r="BK10" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL10" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN10" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BP10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BQ10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BR10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW10" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BX10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CA10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CB10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CC10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CD10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG10" s="239"/>
       <c r="CH10" s="239"/>
@@ -52718,249 +52806,249 @@
       <c r="CQ10" s="239"/>
       <c r="CR10" s="239"/>
       <c r="CS10" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="236" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B11" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J11" s="239" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="K11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="L11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="N11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O11" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P11" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="S11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="T11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="U11" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="V11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Y11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AB11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AC11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AE11" s="243"/>
       <c r="AF11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AG11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AH11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AI11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL11" s="243"/>
       <c r="AM11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AN11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AO11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AP11" s="243"/>
       <c r="AQ11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AR11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AS11" s="243"/>
       <c r="AT11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AU11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AV11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AW11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AY11" s="243"/>
       <c r="AZ11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BA11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BB11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BC11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BE11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BF11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BG11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BH11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI11" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BJ11" s="243"/>
       <c r="BK11" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BL11" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BM11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN11" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BP11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BQ11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BR11" s="239" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="BS11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BT11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BU11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BX11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BY11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CA11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CB11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CC11" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CD11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG11" s="239"/>
       <c r="CH11" s="239"/>
@@ -52975,249 +53063,249 @@
       <c r="CQ11" s="239"/>
       <c r="CR11" s="239"/>
       <c r="CS11" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="236" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B12" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="L12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="N12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="O12" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P12" s="240" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="R12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="S12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="T12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="U12" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="V12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="W12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="X12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Y12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Z12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AB12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AC12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AE12" s="243"/>
       <c r="AF12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AG12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AH12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AI12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AJ12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AK12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AL12" s="243"/>
       <c r="AM12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AN12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AO12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AP12" s="243"/>
       <c r="AQ12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AR12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AS12" s="243"/>
       <c r="AT12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AU12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AV12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AW12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AX12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AY12" s="243"/>
       <c r="AZ12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BA12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BB12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BC12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BD12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BE12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BF12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BG12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BH12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BI12" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BJ12" s="243"/>
       <c r="BK12" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BL12" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BM12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BN12" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BO12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BP12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BQ12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BR12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BS12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BT12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BU12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BV12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BX12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BY12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BZ12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CA12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CB12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CC12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CD12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CE12" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CG12" s="239"/>
       <c r="CH12" s="239"/>
@@ -53232,249 +53320,249 @@
       <c r="CQ12" s="239"/>
       <c r="CR12" s="239"/>
       <c r="CS12" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="236" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B13" s="237" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="L13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="M13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="O13" s="239" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P13" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Q13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="R13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="S13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="T13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="U13" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="V13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="W13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="X13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Y13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Z13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AA13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AB13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AC13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AD13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AE13" s="245"/>
       <c r="AF13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AG13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AH13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AI13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AJ13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AK13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AL13" s="245"/>
       <c r="AM13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AN13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AO13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AP13" s="245"/>
       <c r="AQ13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AR13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AS13" s="245"/>
       <c r="AT13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AU13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AV13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AW13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AX13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AY13" s="245"/>
       <c r="AZ13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BA13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BB13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BC13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BD13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BE13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BF13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BG13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BH13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BI13" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BJ13" s="245"/>
       <c r="BK13" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BL13" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BM13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BN13" s="240" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BO13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BP13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BQ13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BR13" s="239" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="BS13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BT13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BU13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BV13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BW13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BX13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BY13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BZ13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CA13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CB13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CC13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="CD13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CE13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CF13" s="239" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="CG13" s="239"/>
       <c r="CH13" s="239"/>
@@ -53489,7 +53577,7 @@
       <c r="CQ13" s="239"/>
       <c r="CR13" s="239"/>
       <c r="CS13" s="239" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54515,7 +54603,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="246" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B1" s="246" t="s">
         <v>2</v>
@@ -54542,13 +54630,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="250" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="K1" s="251" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="L1" s="249" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M1" s="252"/>
       <c r="N1" s="252"/>
@@ -54567,10 +54655,10 @@
     </row>
     <row r="2">
       <c r="A2" s="253" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B2" s="254" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C2" s="255"/>
       <c r="D2" s="255" t="s">
@@ -54597,7 +54685,7 @@
       </c>
       <c r="K2" s="258"/>
       <c r="L2" s="259" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="M2" s="252"/>
       <c r="N2" s="252"/>
@@ -54616,16 +54704,16 @@
     </row>
     <row r="3">
       <c r="A3" s="253" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B3" s="260" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C3" s="261" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D3" s="255" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E3" s="256">
         <v>45575.0</v>
@@ -54644,7 +54732,7 @@
       </c>
       <c r="K3" s="256"/>
       <c r="L3" s="259" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="M3" s="262"/>
       <c r="N3" s="252"/>
@@ -54663,14 +54751,14 @@
     </row>
     <row r="4">
       <c r="A4" s="253" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B4" s="243"/>
       <c r="C4" s="263" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D4" s="255" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E4" s="256">
         <v>45575.0</v>
@@ -54689,7 +54777,7 @@
       </c>
       <c r="K4" s="264"/>
       <c r="L4" s="267" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="M4" s="262"/>
       <c r="N4" s="252"/>
@@ -54708,16 +54796,16 @@
     </row>
     <row r="5">
       <c r="A5" s="253" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B5" s="249" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="255" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" s="255" t="s">
         <v>233</v>
-      </c>
-      <c r="C5" s="255" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="255" t="s">
-        <v>229</v>
       </c>
       <c r="E5" s="256">
         <v>45575.0</v>
@@ -54736,7 +54824,7 @@
       </c>
       <c r="K5" s="256"/>
       <c r="L5" s="259" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="M5" s="262"/>
       <c r="N5" s="252"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 15 de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_proteccion.xlsx
+++ b/Segumiento_proteccion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="249">
   <si>
     <t>Asignado a</t>
   </si>
@@ -437,6 +437,36 @@
   </si>
   <si>
     <t>Generación de servicio para el tratamiento de datos usando agentes</t>
+  </si>
+  <si>
+    <t>12/09/2025 Desde el día Mierrcoles 10 de sep no se avanza debido a que se debía de trabajar en requerimientos de mayor impórtancia para el cliente</t>
+  </si>
+  <si>
+    <t>Interno2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se identificaron, a través de un informe recién creado que había un hueco en la información. </t>
+  </si>
+  <si>
+    <t>Corrección de datos guardados en BD</t>
+  </si>
+  <si>
+    <t>12/09/2025 Se identifica los datos, se correlacionan entre sí y se completa 3000 datos de 4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se identificaron, a través de un informe recién creado que había un hueco en la información que debe ser corregido. </t>
+  </si>
+  <si>
+    <t>REQ-10-1</t>
+  </si>
+  <si>
+    <t>Se necesita la descarga de imagenes según varios filtros y necesidades del usuario</t>
+  </si>
+  <si>
+    <t>Descarga de archivos relacionados a un cargue de datos, que identifican tipo de documento, año y a quien pertenece</t>
+  </si>
+  <si>
+    <t>12/09/2025 Se realiza la descarga y se esta en la espera de habilitación del punto de carga. Además, se indica que se debe de hacer un proceso de descarga adicional</t>
   </si>
   <si>
     <t>Alejandro Cardona Ocampo</t>
@@ -1946,14 +1976,14 @@
     <xf borderId="3" fillId="6" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="6" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="6" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="9" fillId="6" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3962,7 +3992,7 @@
       <c r="L20" s="82"/>
       <c r="M20" s="24">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N20" s="56"/>
       <c r="O20" s="57"/>
@@ -3997,7 +4027,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="39">
         <f>IF(ISBLANK(L21), NETWORKDAYS(I20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(I20, L21, Hoja2!$A$1:$A$18))</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N21" s="72"/>
       <c r="O21" s="60"/>
@@ -4089,7 +4119,7 @@
       <c r="L23" s="85"/>
       <c r="M23" s="39">
         <f>IF(ISBLANK(L23), NETWORKDAYS(J23, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J23, L23, Hoja2!$A$1:$A$18))</f>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N23" s="72"/>
       <c r="O23" s="60"/>
@@ -4275,7 +4305,7 @@
       <c r="L27" s="85"/>
       <c r="M27" s="39">
         <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
-        <v>32778</v>
+        <v>32780</v>
       </c>
       <c r="N27" s="72"/>
       <c r="O27" s="60"/>
@@ -4549,49 +4579,179 @@
       <c r="L33" s="71"/>
       <c r="M33" s="39">
         <f>IF(ISBLANK(L33), NETWORKDAYS(J33, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J33, L33, Hoja2!$A$1:$A$18))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N33" s="71"/>
       <c r="O33" s="60"/>
-      <c r="P33" s="96"/>
+      <c r="P33" s="96" t="s">
+        <v>119</v>
+      </c>
       <c r="Q33" s="43" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="97"/>
-      <c r="G34" s="98"/>
-      <c r="Q34" s="99"/>
+      <c r="A34" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="77">
+        <v>100.0</v>
+      </c>
+      <c r="H34" s="65">
+        <v>2.0</v>
+      </c>
+      <c r="I34" s="66">
+        <v>45909.0</v>
+      </c>
+      <c r="J34" s="66">
+        <v>45910.0</v>
+      </c>
+      <c r="K34" s="67">
+        <v>45911.0</v>
+      </c>
+      <c r="L34" s="67">
+        <v>45911.0</v>
+      </c>
+      <c r="M34" s="24">
+        <f>IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
+        <v>2</v>
+      </c>
+      <c r="N34" s="67">
+        <v>45911.0</v>
+      </c>
+      <c r="O34" s="57"/>
+      <c r="P34" s="95" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q34" s="28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
-      <c r="B35" s="100"/>
-      <c r="G35" s="101"/>
-      <c r="Q35" s="102"/>
+      <c r="A35" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="90">
+        <v>100.0</v>
+      </c>
+      <c r="H35" s="48">
+        <v>2.0</v>
+      </c>
+      <c r="I35" s="54">
+        <v>45909.0</v>
+      </c>
+      <c r="J35" s="54">
+        <v>45910.0</v>
+      </c>
+      <c r="K35" s="71">
+        <v>45911.0</v>
+      </c>
+      <c r="L35" s="71">
+        <v>45911.0</v>
+      </c>
+      <c r="M35" s="39">
+        <f>IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
+        <v>2</v>
+      </c>
+      <c r="N35" s="71">
+        <v>45911.0</v>
+      </c>
+      <c r="O35" s="60"/>
+      <c r="P35" s="96" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q35" s="43" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
-      <c r="B36" s="97"/>
-      <c r="G36" s="98"/>
-      <c r="Q36" s="99"/>
+      <c r="A36" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" s="77">
+        <v>80.0</v>
+      </c>
+      <c r="H36" s="65">
+        <v>4.0</v>
+      </c>
+      <c r="I36" s="66">
+        <v>45909.0</v>
+      </c>
+      <c r="J36" s="66">
+        <v>45910.0</v>
+      </c>
+      <c r="K36" s="67">
+        <v>45915.0</v>
+      </c>
+      <c r="L36" s="67"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="95" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q36" s="28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
-      <c r="B37" s="100"/>
-      <c r="G37" s="101"/>
-      <c r="Q37" s="102"/>
+      <c r="B37" s="97"/>
+      <c r="G37" s="98"/>
+      <c r="Q37" s="99"/>
     </row>
     <row r="38">
-      <c r="B38" s="97"/>
-      <c r="G38" s="98"/>
-      <c r="Q38" s="99"/>
+      <c r="B38" s="100"/>
+      <c r="G38" s="101"/>
+      <c r="Q38" s="102"/>
     </row>
     <row r="39">
-      <c r="B39" s="100"/>
-      <c r="G39" s="101"/>
-      <c r="Q39" s="102"/>
+      <c r="B39" s="97"/>
+      <c r="G39" s="98"/>
+      <c r="Q39" s="99"/>
     </row>
     <row r="40">
-      <c r="B40" s="97"/>
-      <c r="G40" s="98"/>
-      <c r="Q40" s="99"/>
+      <c r="B40" s="100"/>
+      <c r="G40" s="101"/>
+      <c r="Q40" s="102"/>
     </row>
     <row r="41" ht="29.25" customHeight="1">
       <c r="A41" s="103"/>
@@ -41501,10 +41661,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L20 I21 K21:L21 I22:L33 N2:O33 I41:L940 N41:O940">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L20 I21 K21:L21 I22:L36 N2:O36 I41:L940 N41:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F33 F41:F940">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F36 F41:F940">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -41602,19 +41762,19 @@
     </row>
     <row r="2" ht="29.25" customHeight="1">
       <c r="A2" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B2" s="144" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="145" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D2" s="144" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="144" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="F2" s="146" t="s">
         <v>21</v>
@@ -41649,19 +41809,19 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B3" s="144" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="145" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D3" s="144" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F3" s="146" t="s">
         <v>21</v>
@@ -41696,19 +41856,19 @@
     </row>
     <row r="4" ht="39.0" customHeight="1">
       <c r="A4" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B4" s="144" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="145" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D4" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="144" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F4" s="146" t="s">
         <v>21</v>
@@ -41747,19 +41907,19 @@
     </row>
     <row r="5">
       <c r="A5" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B5" s="144" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D5" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="160" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F5" s="146" t="s">
         <v>21</v>
@@ -41798,19 +41958,19 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B6" s="144" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="145" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D6" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="162" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F6" s="163" t="s">
         <v>21</v>
@@ -41849,19 +42009,19 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B7" s="144" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="145" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D7" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="144" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="F7" s="165" t="s">
         <v>21</v>
@@ -41900,19 +42060,19 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B8" s="144" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="145" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D8" s="144" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="167" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="F8" s="146" t="s">
         <v>21</v>
@@ -41947,17 +42107,17 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B9" s="144" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="171" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D9" s="172"/>
       <c r="E9" s="144" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="F9" s="165" t="s">
         <v>21</v>
@@ -41994,17 +42154,17 @@
     </row>
     <row r="10" ht="93.0" customHeight="1">
       <c r="A10" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B10" s="144" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="171" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D10" s="172"/>
       <c r="E10" s="144" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="F10" s="165" t="s">
         <v>21</v>
@@ -42039,19 +42199,19 @@
     </row>
     <row r="11">
       <c r="A11" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B11" s="144" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="145" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D11" s="144" t="s">
         <v>41</v>
       </c>
       <c r="E11" s="174" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F11" s="165" t="s">
         <v>21</v>
@@ -42088,19 +42248,19 @@
     </row>
     <row r="12" ht="29.25" customHeight="1">
       <c r="A12" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B12" s="144" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="175" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D12" s="144" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="144" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="F12" s="165" t="s">
         <v>21</v>
@@ -42137,19 +42297,19 @@
     </row>
     <row r="13" ht="29.25" customHeight="1">
       <c r="A13" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B13" s="144" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="171" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D13" s="144" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="144" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="F13" s="165" t="s">
         <v>21</v>
@@ -42184,7 +42344,7 @@
     </row>
     <row r="14" ht="29.25" customHeight="1">
       <c r="A14" s="143" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B14" s="144" t="s">
         <v>60</v>
@@ -42194,7 +42354,7 @@
       </c>
       <c r="D14" s="176"/>
       <c r="E14" s="162" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F14" s="170" t="s">
         <v>21</v>
@@ -42272,7 +42432,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="177" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B1" s="177" t="s">
         <v>2</v>
@@ -42299,13 +42459,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="180" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="K1" s="177" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="L1" s="181" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="M1" s="182"/>
       <c r="N1" s="182"/>
@@ -42324,14 +42484,14 @@
     </row>
     <row r="2">
       <c r="A2" s="183" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B2" s="184" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C2" s="185"/>
       <c r="D2" s="186" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E2" s="187">
         <v>45526.0</v>
@@ -42345,7 +42505,7 @@
       <c r="J2" s="185"/>
       <c r="K2" s="185"/>
       <c r="L2" s="185" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="M2" s="188"/>
       <c r="N2" s="188"/>
@@ -42364,13 +42524,13 @@
     </row>
     <row r="3">
       <c r="A3" s="189" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B3" s="190" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C3" s="191" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D3" s="191" t="s">
         <v>21</v>
@@ -42394,7 +42554,7 @@
       </c>
       <c r="K3" s="193"/>
       <c r="L3" s="195" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="M3" s="182"/>
       <c r="N3" s="182"/>
@@ -42413,16 +42573,16 @@
     </row>
     <row r="4">
       <c r="A4" s="196" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B4" s="197" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C4" s="196" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D4" s="198" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E4" s="199">
         <v>45581.0</v>
@@ -42445,7 +42605,7 @@
       </c>
       <c r="K4" s="199"/>
       <c r="L4" s="196" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="M4" s="202"/>
       <c r="N4" s="202"/>
@@ -42464,13 +42624,13 @@
     </row>
     <row r="5">
       <c r="A5" s="181" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B5" s="197" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C5" s="191" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D5" s="203" t="s">
         <v>65</v>
@@ -42494,7 +42654,7 @@
       </c>
       <c r="K5" s="192"/>
       <c r="L5" s="195" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="M5" s="182"/>
       <c r="N5" s="182"/>
@@ -42513,16 +42673,16 @@
     </row>
     <row r="6">
       <c r="A6" s="204" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B6" s="204" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C6" s="198" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D6" s="204" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E6" s="205">
         <v>45602.0</v>
@@ -42543,7 +42703,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="206" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="M6" s="207"/>
       <c r="N6" s="208"/>
@@ -42562,13 +42722,13 @@
     </row>
     <row r="7">
       <c r="A7" s="181" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B7" s="190" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C7" s="209" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D7" s="203" t="s">
         <v>65</v>
@@ -42592,7 +42752,7 @@
       </c>
       <c r="K7" s="203"/>
       <c r="L7" s="211" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="M7" s="212"/>
       <c r="N7" s="212"/>
@@ -42611,14 +42771,14 @@
     </row>
     <row r="8">
       <c r="A8" s="213" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B8" s="214" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C8" s="215"/>
       <c r="D8" s="215" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E8" s="216">
         <v>45603.0</v>
@@ -42639,7 +42799,7 @@
       </c>
       <c r="K8" s="216"/>
       <c r="L8" s="218" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="M8" s="182"/>
       <c r="N8" s="182"/>
@@ -42658,16 +42818,16 @@
     </row>
     <row r="9">
       <c r="A9" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B9" s="220" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C9" s="221" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D9" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E9" s="223">
         <v>45671.0</v>
@@ -42676,7 +42836,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="221" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="H9" s="223">
         <v>45680.0</v>
@@ -42690,7 +42850,7 @@
       </c>
       <c r="K9" s="221"/>
       <c r="L9" s="225" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="M9" s="226"/>
       <c r="N9" s="226"/>
@@ -42709,14 +42869,14 @@
     </row>
     <row r="10">
       <c r="A10" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B10" s="227"/>
       <c r="C10" s="225" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D10" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E10" s="223">
         <v>45671.0</v>
@@ -42735,7 +42895,7 @@
       <c r="J10" s="221"/>
       <c r="K10" s="221"/>
       <c r="L10" s="225" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="M10" s="226"/>
       <c r="N10" s="226"/>
@@ -42754,14 +42914,14 @@
     </row>
     <row r="11">
       <c r="A11" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B11" s="227"/>
       <c r="C11" s="225" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="D11" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E11" s="223">
         <v>45671.0</v>
@@ -42780,7 +42940,7 @@
       <c r="J11" s="221"/>
       <c r="K11" s="221"/>
       <c r="L11" s="225" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="M11" s="226"/>
       <c r="N11" s="226"/>
@@ -42799,14 +42959,14 @@
     </row>
     <row r="12">
       <c r="A12" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B12" s="227"/>
       <c r="C12" s="225" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D12" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E12" s="223">
         <v>45671.0</v>
@@ -42825,7 +42985,7 @@
       <c r="J12" s="221"/>
       <c r="K12" s="221"/>
       <c r="L12" s="225" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="M12" s="226"/>
       <c r="N12" s="226"/>
@@ -42844,14 +43004,14 @@
     </row>
     <row r="13">
       <c r="A13" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B13" s="227"/>
       <c r="C13" s="225" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D13" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E13" s="223">
         <v>45671.0</v>
@@ -42870,7 +43030,7 @@
       <c r="J13" s="221"/>
       <c r="K13" s="221"/>
       <c r="L13" s="225" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="M13" s="226"/>
       <c r="N13" s="226"/>
@@ -42889,14 +43049,14 @@
     </row>
     <row r="14">
       <c r="A14" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B14" s="227"/>
       <c r="C14" s="225" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D14" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E14" s="223">
         <v>45671.0</v>
@@ -42915,7 +43075,7 @@
       <c r="J14" s="221"/>
       <c r="K14" s="221"/>
       <c r="L14" s="221" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="M14" s="226"/>
       <c r="N14" s="226"/>
@@ -42934,14 +43094,14 @@
     </row>
     <row r="15">
       <c r="A15" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B15" s="227"/>
       <c r="C15" s="225" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="222" t="s">
         <v>182</v>
-      </c>
-      <c r="D15" s="222" t="s">
-        <v>172</v>
       </c>
       <c r="E15" s="223">
         <v>45671.0</v>
@@ -42960,7 +43120,7 @@
       <c r="J15" s="221"/>
       <c r="K15" s="221"/>
       <c r="L15" s="221" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="M15" s="226"/>
       <c r="N15" s="226"/>
@@ -42979,14 +43139,14 @@
     </row>
     <row r="16">
       <c r="A16" s="219" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B16" s="228"/>
       <c r="C16" s="229" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D16" s="222" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E16" s="223">
         <v>45681.0</v>
@@ -43005,7 +43165,7 @@
       <c r="J16" s="221"/>
       <c r="K16" s="221"/>
       <c r="L16" s="225" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="M16" s="226"/>
       <c r="N16" s="226"/>
@@ -49541,7 +49701,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="226" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49549,7 +49709,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="226" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49557,7 +49717,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="226" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49565,7 +49725,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="226" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49573,7 +49733,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="226" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49581,7 +49741,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="226" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49589,7 +49749,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="226" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49597,7 +49757,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="226" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49605,7 +49765,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="226" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49613,7 +49773,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="226" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49621,7 +49781,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="226" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49629,7 +49789,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="226" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49637,7 +49797,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="226" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49645,7 +49805,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="226" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49653,7 +49813,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="226" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49661,7 +49821,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="226" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49669,7 +49829,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="226" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49677,7 +49837,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="226" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50693,7 +50853,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="231" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B1" s="226"/>
       <c r="C1" s="226"/>
@@ -50751,7 +50911,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="232" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B3" s="233">
         <v>45596.0</v>
@@ -51044,261 +51204,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="236" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B4" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C4" s="238" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="D4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="J4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="L4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="M4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="O4" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P4" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U4" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="V4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE4" s="241" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="AF4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL4" s="241" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="AM4" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AN4" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AO4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP4" s="241" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="AQ4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS4" s="241" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="AT4" s="242" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AV4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY4" s="241" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="AZ4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BA4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BH4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI4" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ4" s="241" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="BK4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BL4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BM4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BN4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BO4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BP4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BQ4" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BR4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CA4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CB4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CC4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CD4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG4" s="239"/>
       <c r="CH4" s="239"/>
       <c r="CI4" s="241" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="CJ4" s="239"/>
       <c r="CK4" s="239"/>
@@ -51310,249 +51470,249 @@
       <c r="CQ4" s="239"/>
       <c r="CR4" s="239"/>
       <c r="CS4" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="236" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B5" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="J5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="L5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="M5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="N5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="O5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="P5" s="240" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="Q5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U5" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="V5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE5" s="243"/>
       <c r="AF5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL5" s="243"/>
       <c r="AM5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AN5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AO5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP5" s="243"/>
       <c r="AQ5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AR5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AS5" s="243"/>
       <c r="AT5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AU5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AV5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AW5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AX5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="AY5" s="243"/>
       <c r="AZ5" s="239" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BA5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BH5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI5" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ5" s="243"/>
       <c r="BK5" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL5" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN5" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BO5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BP5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BQ5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BR5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CA5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CB5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CC5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CD5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG5" s="239"/>
       <c r="CH5" s="239"/>
@@ -51567,249 +51727,249 @@
       <c r="CQ5" s="239"/>
       <c r="CR5" s="239"/>
       <c r="CS5" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="236" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B6" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="J6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K6" s="244" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="L6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="M6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="O6" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P6" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U6" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="V6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE6" s="243"/>
       <c r="AF6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL6" s="243"/>
       <c r="AM6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AN6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AO6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP6" s="243"/>
       <c r="AQ6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS6" s="243"/>
       <c r="AT6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AV6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY6" s="243"/>
       <c r="AZ6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BA6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BH6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI6" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ6" s="243"/>
       <c r="BK6" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL6" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM6" s="239" t="s">
+        <v>225</v>
+      </c>
+      <c r="BN6" s="240" t="s">
         <v>215</v>
       </c>
-      <c r="BN6" s="240" t="s">
-        <v>205</v>
-      </c>
       <c r="BO6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BP6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BQ6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BR6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CA6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CB6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CC6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CD6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG6" s="239"/>
       <c r="CH6" s="239"/>
@@ -51824,198 +51984,198 @@
       <c r="CQ6" s="239"/>
       <c r="CR6" s="239"/>
       <c r="CS6" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="236" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B7" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="J7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="L7" s="244" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="M7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="O7" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P7" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U7" s="240" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="V7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z7" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AA7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE7" s="243"/>
       <c r="AF7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL7" s="243"/>
       <c r="AM7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AN7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AO7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP7" s="243"/>
       <c r="AQ7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS7" s="243"/>
       <c r="AT7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU7" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AV7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY7" s="243"/>
       <c r="AZ7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BA7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BH7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI7" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ7" s="243"/>
       <c r="BK7" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL7" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN7" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BO7" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BP7" s="239"/>
       <c r="BQ7" s="239"/>
@@ -52023,16 +52183,16 @@
       <c r="BS7" s="239"/>
       <c r="BT7" s="239"/>
       <c r="BU7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX7" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY7" s="239"/>
       <c r="BZ7" s="239"/>
@@ -52058,220 +52218,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="236" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="237" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="I8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="J8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" s="239" t="s">
+        <v>215</v>
+      </c>
+      <c r="L8" s="239" t="s">
         <v>218</v>
       </c>
-      <c r="B8" s="237" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="D8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="G8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="H8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="I8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="J8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="K8" s="239" t="s">
-        <v>205</v>
-      </c>
-      <c r="L8" s="239" t="s">
-        <v>208</v>
-      </c>
       <c r="M8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="O8" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P8" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U8" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="V8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W8" s="239" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="X8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB8" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AC8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE8" s="243"/>
       <c r="AF8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL8" s="243"/>
       <c r="AM8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AN8" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AO8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP8" s="243"/>
       <c r="AQ8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS8" s="243"/>
       <c r="AT8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AV8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY8" s="243"/>
       <c r="AZ8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BA8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG8" s="239" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="BH8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI8" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ8" s="243"/>
       <c r="BK8" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL8" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN8" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BO8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BP8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BQ8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BR8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW8" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX8" s="239" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="BY8" s="239"/>
       <c r="BZ8" s="239"/>
@@ -52297,244 +52457,244 @@
     </row>
     <row r="9">
       <c r="A9" s="236" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B9" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="J9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="L9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="M9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="O9" s="244" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="P9" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U9" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="V9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE9" s="243"/>
       <c r="AF9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL9" s="243"/>
       <c r="AM9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AN9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AO9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP9" s="243"/>
       <c r="AQ9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS9" s="243"/>
       <c r="AT9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AV9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY9" s="243"/>
       <c r="AZ9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BA9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BH9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI9" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ9" s="243"/>
       <c r="BK9" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL9" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN9" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BO9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BP9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BQ9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BR9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CA9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CB9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CC9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CD9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG9" s="239"/>
       <c r="CH9" s="239"/>
@@ -52549,249 +52709,249 @@
       <c r="CQ9" s="239"/>
       <c r="CR9" s="239"/>
       <c r="CS9" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="236" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B10" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="J10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="L10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="M10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="O10" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P10" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Q10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="R10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="T10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="U10" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="V10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AE10" s="243"/>
       <c r="AF10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AL10" s="243"/>
       <c r="AM10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AN10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AO10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP10" s="243"/>
       <c r="AQ10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS10" s="243"/>
       <c r="AT10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AV10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY10" s="243"/>
       <c r="AZ10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BA10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BB10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BC10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BD10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BE10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BF10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BG10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BH10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI10" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ10" s="243"/>
       <c r="BK10" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL10" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN10" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BO10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BP10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BQ10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BR10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW10" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BX10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CA10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CB10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CC10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CD10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG10" s="239"/>
       <c r="CH10" s="239"/>
@@ -52806,249 +52966,249 @@
       <c r="CQ10" s="239"/>
       <c r="CR10" s="239"/>
       <c r="CS10" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="236" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="B11" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="J11" s="239" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="K11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="L11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="M11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="N11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="O11" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P11" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="R11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="S11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="T11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="U11" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="V11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Y11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Z11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AB11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AC11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AE11" s="243"/>
       <c r="AF11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AG11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AH11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AI11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL11" s="243"/>
       <c r="AM11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AN11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AO11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AP11" s="243"/>
       <c r="AQ11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AR11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AS11" s="243"/>
       <c r="AT11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AU11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AV11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AW11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AY11" s="243"/>
       <c r="AZ11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BA11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BB11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BC11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BE11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BF11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BG11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BH11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI11" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ11" s="243"/>
       <c r="BK11" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BL11" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BM11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN11" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BO11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BP11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BQ11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BR11" s="239" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="BS11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BT11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BU11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BX11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BY11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CA11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CB11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CC11" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CD11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG11" s="239"/>
       <c r="CH11" s="239"/>
@@ -53063,249 +53223,249 @@
       <c r="CQ11" s="239"/>
       <c r="CR11" s="239"/>
       <c r="CS11" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="236" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B12" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="D12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="H12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="J12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="L12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="M12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="N12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="O12" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P12" s="240" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="Q12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="R12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="S12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="T12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="U12" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="V12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="W12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="X12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Y12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Z12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AA12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AB12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AC12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AE12" s="243"/>
       <c r="AF12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AG12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AH12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AI12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AJ12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AK12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AL12" s="243"/>
       <c r="AM12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AN12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AO12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AP12" s="243"/>
       <c r="AQ12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AR12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AS12" s="243"/>
       <c r="AT12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AU12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AV12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AW12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AX12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AY12" s="243"/>
       <c r="AZ12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BA12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BB12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BC12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BD12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BE12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BF12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BG12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BH12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BI12" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BJ12" s="243"/>
       <c r="BK12" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BL12" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BM12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BN12" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BO12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BP12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BQ12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BR12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BS12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BT12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BU12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BV12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BW12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BX12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BY12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BZ12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CA12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CB12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CC12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CD12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CE12" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CG12" s="239"/>
       <c r="CH12" s="239"/>
@@ -53320,249 +53480,249 @@
       <c r="CQ12" s="239"/>
       <c r="CR12" s="239"/>
       <c r="CS12" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="236" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B13" s="237" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="D13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="E13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="F13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="H13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="I13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="J13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="L13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="M13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="O13" s="239" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P13" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Q13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="R13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="S13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="T13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="U13" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="V13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="W13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="X13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Y13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Z13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AA13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AB13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AC13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AD13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AE13" s="245"/>
       <c r="AF13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AG13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AH13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AI13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="AJ13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AK13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AL13" s="245"/>
       <c r="AM13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AN13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AO13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AP13" s="245"/>
       <c r="AQ13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AR13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AS13" s="245"/>
       <c r="AT13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AU13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AV13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AW13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AX13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="AY13" s="245"/>
       <c r="AZ13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BA13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BB13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BC13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BD13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BE13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BF13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BG13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BH13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BI13" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BJ13" s="245"/>
       <c r="BK13" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BL13" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BM13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BN13" s="240" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BO13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BP13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BQ13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BR13" s="239" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="BS13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BT13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BU13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BV13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BW13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BX13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BY13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BZ13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CA13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CB13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CC13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="CD13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CE13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CF13" s="239" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="CG13" s="239"/>
       <c r="CH13" s="239"/>
@@ -53577,7 +53737,7 @@
       <c r="CQ13" s="239"/>
       <c r="CR13" s="239"/>
       <c r="CS13" s="239" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54603,7 +54763,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="246" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B1" s="246" t="s">
         <v>2</v>
@@ -54630,13 +54790,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="250" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="K1" s="251" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="L1" s="249" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="M1" s="252"/>
       <c r="N1" s="252"/>
@@ -54655,10 +54815,10 @@
     </row>
     <row r="2">
       <c r="A2" s="253" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B2" s="254" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="C2" s="255"/>
       <c r="D2" s="255" t="s">
@@ -54685,7 +54845,7 @@
       </c>
       <c r="K2" s="258"/>
       <c r="L2" s="259" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="M2" s="252"/>
       <c r="N2" s="252"/>
@@ -54704,16 +54864,16 @@
     </row>
     <row r="3">
       <c r="A3" s="253" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B3" s="260" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C3" s="261" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="D3" s="255" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="E3" s="256">
         <v>45575.0</v>
@@ -54732,7 +54892,7 @@
       </c>
       <c r="K3" s="256"/>
       <c r="L3" s="259" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="M3" s="262"/>
       <c r="N3" s="252"/>
@@ -54751,14 +54911,14 @@
     </row>
     <row r="4">
       <c r="A4" s="253" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B4" s="243"/>
       <c r="C4" s="263" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="D4" s="255" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="E4" s="256">
         <v>45575.0</v>
@@ -54777,7 +54937,7 @@
       </c>
       <c r="K4" s="264"/>
       <c r="L4" s="267" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="M4" s="262"/>
       <c r="N4" s="252"/>
@@ -54796,16 +54956,16 @@
     </row>
     <row r="5">
       <c r="A5" s="253" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B5" s="249" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="C5" s="255" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="D5" s="255" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="E5" s="256">
         <v>45575.0</v>
@@ -54824,7 +54984,7 @@
       </c>
       <c r="K5" s="256"/>
       <c r="L5" s="259" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="M5" s="262"/>
       <c r="N5" s="252"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 19 de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_proteccion.xlsx
+++ b/Segumiento_proteccion.xlsx
@@ -439,7 +439,8 @@
     <t>Generación de servicio para el tratamiento de datos usando agentes</t>
   </si>
   <si>
-    <t>12/09/2025 Desde el día Mierrcoles 10 de sep no se avanza debido a que se debía de trabajar en requerimientos de mayor impórtancia para el cliente</t>
+    <t>12/09/2025 Desde el día Mierrcoles 10 de sep no se avanza debido a que se debía de trabajar en requerimientos de mayor impórtancia para el cliente
+19/09/2025 Se volvio a retomar el días 15 en la tarde, cuando se termina los pendientes de mayor importancia, terminando sus pruebas el 18</t>
   </si>
   <si>
     <t>Interno2-1</t>
@@ -466,7 +467,8 @@
     <t>Descarga de archivos relacionados a un cargue de datos, que identifican tipo de documento, año y a quien pertenece</t>
   </si>
   <si>
-    <t>12/09/2025 Se realiza la descarga y se esta en la espera de habilitación del punto de carga. Además, se indica que se debe de hacer un proceso de descarga adicional</t>
+    <t>12/09/2025 Se realiza la descarga y se esta en la espera de habilitación del punto de carga. Además, se indica que se debe de hacer un proceso de descarga adicional
+19/09/2025 Se han realizado reuniones a lo largo de la semana para la habilitación de un punto de cargue por parte del cliente</t>
   </si>
   <si>
     <t>Alejandro Cardona Ocampo</t>
@@ -3831,7 +3833,7 @@
         <v>65</v>
       </c>
       <c r="G17" s="34">
-        <v>50.0</v>
+        <v>99.0</v>
       </c>
       <c r="H17" s="35">
         <v>2.0</v>
@@ -3992,7 +3994,7 @@
       <c r="L20" s="82"/>
       <c r="M20" s="24">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N20" s="56"/>
       <c r="O20" s="57"/>
@@ -4027,7 +4029,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="39">
         <f>IF(ISBLANK(L21), NETWORKDAYS(I20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(I20, L21, Hoja2!$A$1:$A$18))</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N21" s="72"/>
       <c r="O21" s="60"/>
@@ -4119,7 +4121,7 @@
       <c r="L23" s="85"/>
       <c r="M23" s="39">
         <f>IF(ISBLANK(L23), NETWORKDAYS(J23, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J23, L23, Hoja2!$A$1:$A$18))</f>
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="N23" s="72"/>
       <c r="O23" s="60"/>
@@ -4305,7 +4307,7 @@
       <c r="L27" s="85"/>
       <c r="M27" s="39">
         <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
-        <v>32780</v>
+        <v>32784</v>
       </c>
       <c r="N27" s="72"/>
       <c r="O27" s="60"/>
@@ -4314,7 +4316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="138.0" customHeight="1">
       <c r="A28" s="15" t="s">
         <v>17</v>
       </c>
@@ -4329,8 +4331,8 @@
       <c r="F28" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="77">
-        <v>50.0</v>
+      <c r="G28" s="20">
+        <v>99.0</v>
       </c>
       <c r="H28" s="65">
         <v>4.0</v>
@@ -4425,8 +4427,8 @@
       <c r="F30" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="77">
-        <v>50.0</v>
+      <c r="G30" s="20">
+        <v>99.0</v>
       </c>
       <c r="H30" s="65">
         <v>5.0</v>
@@ -4471,8 +4473,8 @@
       <c r="F31" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="90">
-        <v>50.0</v>
+      <c r="G31" s="34">
+        <v>99.0</v>
       </c>
       <c r="H31" s="48">
         <v>3.0</v>
@@ -4546,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" ht="76.5" customHeight="1">
       <c r="A33" s="29" t="s">
         <v>17</v>
       </c>
@@ -4559,10 +4561,10 @@
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="86" t="s">
-        <v>91</v>
-      </c>
-      <c r="G33" s="90">
-        <v>50.0</v>
+        <v>65</v>
+      </c>
+      <c r="G33" s="34">
+        <v>99.0</v>
       </c>
       <c r="H33" s="48">
         <v>4.0</v>
@@ -4576,12 +4578,16 @@
       <c r="K33" s="71">
         <v>45912.0</v>
       </c>
-      <c r="L33" s="71"/>
+      <c r="L33" s="71">
+        <v>45918.0</v>
+      </c>
       <c r="M33" s="39">
-        <f>IF(ISBLANK(L33), NETWORKDAYS(J33, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J33, L33, Hoja2!$A$1:$A$18))</f>
-        <v>5</v>
-      </c>
-      <c r="N33" s="71"/>
+        <f>IF(ISBLANK(N33), NETWORKDAYS(J33, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J33, N33, Hoja2!$A$1:$A$18))</f>
+        <v>8</v>
+      </c>
+      <c r="N33" s="71">
+        <v>45918.0</v>
+      </c>
       <c r="O33" s="60"/>
       <c r="P33" s="96" t="s">
         <v>119</v>
@@ -4690,7 +4696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="84.75" customHeight="1">
       <c r="A36" s="15" t="s">
         <v>17</v>
       </c>
@@ -4705,10 +4711,10 @@
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="58" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="G36" s="77">
-        <v>80.0</v>
+        <v>99.0</v>
       </c>
       <c r="H36" s="65">
         <v>4.0</v>
@@ -4722,9 +4728,16 @@
       <c r="K36" s="67">
         <v>45915.0</v>
       </c>
-      <c r="L36" s="67"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="67"/>
+      <c r="L36" s="67">
+        <v>45915.0</v>
+      </c>
+      <c r="M36" s="24">
+        <f>IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
+        <v>4</v>
+      </c>
+      <c r="N36" s="67">
+        <v>45915.0</v>
+      </c>
       <c r="O36" s="57"/>
       <c r="P36" s="95" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 25  de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_proteccion.xlsx
+++ b/Segumiento_proteccion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="257">
   <si>
     <t>Asignado a</t>
   </si>
@@ -469,6 +469,32 @@
   <si>
     <t>12/09/2025 Se realiza la descarga y se esta en la espera de habilitación del punto de carga. Además, se indica que se debe de hacer un proceso de descarga adicional
 19/09/2025 Se han realizado reuniones a lo largo de la semana para la habilitación de un punto de cargue por parte del cliente</t>
+  </si>
+  <si>
+    <t>Interno-H13</t>
+  </si>
+  <si>
+    <t>Generación de servicio para el procesamiento de documentos y generación de un documento general</t>
+  </si>
+  <si>
+    <t>Automatización de tarea para el proceso de cambios de fondos de cesantías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/09/2025 Este día solo se trabajo en la migración
+</t>
+  </si>
+  <si>
+    <t>REQ-11-1</t>
+  </si>
+  <si>
+    <t>Se necesita organizar una instancia de AWS, de tal modo que su ambiente quedé diospuesto para funcionar en producción</t>
+  </si>
+  <si>
+    <t>Ambientación de instancia AWS para migración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/09/2025 Se habilitan todos los accesos para el trabajo en el servidor
+</t>
   </si>
   <si>
     <t>Alejandro Cardona Ocampo</t>
@@ -3994,7 +4020,7 @@
       <c r="L20" s="82"/>
       <c r="M20" s="24">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N20" s="56"/>
       <c r="O20" s="57"/>
@@ -4029,7 +4055,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="39">
         <f>IF(ISBLANK(L21), NETWORKDAYS(I20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(I20, L21, Hoja2!$A$1:$A$18))</f>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N21" s="72"/>
       <c r="O21" s="60"/>
@@ -4121,7 +4147,7 @@
       <c r="L23" s="85"/>
       <c r="M23" s="39">
         <f>IF(ISBLANK(L23), NETWORKDAYS(J23, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J23, L23, Hoja2!$A$1:$A$18))</f>
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="N23" s="72"/>
       <c r="O23" s="60"/>
@@ -4307,7 +4333,7 @@
       <c r="L27" s="85"/>
       <c r="M27" s="39">
         <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
-        <v>32784</v>
+        <v>32788</v>
       </c>
       <c r="N27" s="72"/>
       <c r="O27" s="60"/>
@@ -4696,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" ht="84.75" customHeight="1">
+    <row r="36" ht="93.0" customHeight="1">
       <c r="A36" s="15" t="s">
         <v>17</v>
       </c>
@@ -4746,15 +4772,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37">
-      <c r="B37" s="97"/>
-      <c r="G37" s="98"/>
-      <c r="Q37" s="99"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="100"/>
-      <c r="G38" s="101"/>
-      <c r="Q38" s="102"/>
+    <row r="37" ht="76.5" customHeight="1">
+      <c r="A37" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="32"/>
+      <c r="F37" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="34">
+        <v>30.0</v>
+      </c>
+      <c r="H37" s="48">
+        <v>5.0</v>
+      </c>
+      <c r="I37" s="54">
+        <v>45918.0</v>
+      </c>
+      <c r="J37" s="54">
+        <v>45919.0</v>
+      </c>
+      <c r="K37" s="71">
+        <v>45926.0</v>
+      </c>
+      <c r="L37" s="71"/>
+      <c r="M37" s="39">
+        <f>IF(ISBLANK(N37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, N37, Hoja2!$A$1:$A$18))</f>
+        <v>5</v>
+      </c>
+      <c r="N37" s="71"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="96" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q37" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="93.0" customHeight="1">
+      <c r="A38" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="77">
+        <v>30.0</v>
+      </c>
+      <c r="H38" s="65">
+        <v>8.0</v>
+      </c>
+      <c r="I38" s="66">
+        <v>45910.0</v>
+      </c>
+      <c r="J38" s="66">
+        <v>45922.0</v>
+      </c>
+      <c r="K38" s="67">
+        <v>45931.0</v>
+      </c>
+      <c r="L38" s="67"/>
+      <c r="M38" s="24">
+        <f>IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
+        <v>4</v>
+      </c>
+      <c r="N38" s="67"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q38" s="28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" s="97"/>
@@ -41674,10 +41782,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L20 I21 K21:L21 I22:L36 N2:O36 I41:L940 N41:O940">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L20 I21 K21:L21 I22:L38 N2:O38 I41:L940 N41:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F36 F41:F940">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F38 F41:F940">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -41775,19 +41883,19 @@
     </row>
     <row r="2" ht="29.25" customHeight="1">
       <c r="A2" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B2" s="144" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="145" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D2" s="144" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="144" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="F2" s="146" t="s">
         <v>21</v>
@@ -41822,19 +41930,19 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B3" s="144" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="145" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D3" s="144" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F3" s="146" t="s">
         <v>21</v>
@@ -41869,19 +41977,19 @@
     </row>
     <row r="4" ht="39.0" customHeight="1">
       <c r="A4" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B4" s="144" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="145" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D4" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="144" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F4" s="146" t="s">
         <v>21</v>
@@ -41920,19 +42028,19 @@
     </row>
     <row r="5">
       <c r="A5" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B5" s="144" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D5" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="160" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="F5" s="146" t="s">
         <v>21</v>
@@ -41971,19 +42079,19 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B6" s="144" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="145" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D6" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="162" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="F6" s="163" t="s">
         <v>21</v>
@@ -42022,19 +42130,19 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B7" s="144" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="145" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D7" s="144" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="144" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F7" s="165" t="s">
         <v>21</v>
@@ -42073,19 +42181,19 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B8" s="144" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="145" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D8" s="144" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="167" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F8" s="146" t="s">
         <v>21</v>
@@ -42120,17 +42228,17 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B9" s="144" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="171" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D9" s="172"/>
       <c r="E9" s="144" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F9" s="165" t="s">
         <v>21</v>
@@ -42167,17 +42275,17 @@
     </row>
     <row r="10" ht="93.0" customHeight="1">
       <c r="A10" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B10" s="144" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="171" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D10" s="172"/>
       <c r="E10" s="144" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F10" s="165" t="s">
         <v>21</v>
@@ -42212,19 +42320,19 @@
     </row>
     <row r="11">
       <c r="A11" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B11" s="144" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="145" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D11" s="144" t="s">
         <v>41</v>
       </c>
       <c r="E11" s="174" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F11" s="165" t="s">
         <v>21</v>
@@ -42261,19 +42369,19 @@
     </row>
     <row r="12" ht="29.25" customHeight="1">
       <c r="A12" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B12" s="144" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="175" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D12" s="144" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="144" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="F12" s="165" t="s">
         <v>21</v>
@@ -42310,19 +42418,19 @@
     </row>
     <row r="13" ht="29.25" customHeight="1">
       <c r="A13" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B13" s="144" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="171" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D13" s="144" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="144" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F13" s="165" t="s">
         <v>21</v>
@@ -42357,7 +42465,7 @@
     </row>
     <row r="14" ht="29.25" customHeight="1">
       <c r="A14" s="143" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B14" s="144" t="s">
         <v>60</v>
@@ -42367,7 +42475,7 @@
       </c>
       <c r="D14" s="176"/>
       <c r="E14" s="162" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F14" s="170" t="s">
         <v>21</v>
@@ -42445,7 +42553,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="177" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B1" s="177" t="s">
         <v>2</v>
@@ -42472,13 +42580,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="180" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="K1" s="177" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="L1" s="181" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="M1" s="182"/>
       <c r="N1" s="182"/>
@@ -42497,14 +42605,14 @@
     </row>
     <row r="2">
       <c r="A2" s="183" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B2" s="184" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C2" s="185"/>
       <c r="D2" s="186" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E2" s="187">
         <v>45526.0</v>
@@ -42518,7 +42626,7 @@
       <c r="J2" s="185"/>
       <c r="K2" s="185"/>
       <c r="L2" s="185" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="M2" s="188"/>
       <c r="N2" s="188"/>
@@ -42537,13 +42645,13 @@
     </row>
     <row r="3">
       <c r="A3" s="189" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B3" s="190" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C3" s="191" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D3" s="191" t="s">
         <v>21</v>
@@ -42567,7 +42675,7 @@
       </c>
       <c r="K3" s="193"/>
       <c r="L3" s="195" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="M3" s="182"/>
       <c r="N3" s="182"/>
@@ -42586,16 +42694,16 @@
     </row>
     <row r="4">
       <c r="A4" s="196" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B4" s="197" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C4" s="196" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D4" s="198" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E4" s="199">
         <v>45581.0</v>
@@ -42618,7 +42726,7 @@
       </c>
       <c r="K4" s="199"/>
       <c r="L4" s="196" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="M4" s="202"/>
       <c r="N4" s="202"/>
@@ -42637,13 +42745,13 @@
     </row>
     <row r="5">
       <c r="A5" s="181" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B5" s="197" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C5" s="191" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D5" s="203" t="s">
         <v>65</v>
@@ -42667,7 +42775,7 @@
       </c>
       <c r="K5" s="192"/>
       <c r="L5" s="195" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="M5" s="182"/>
       <c r="N5" s="182"/>
@@ -42686,16 +42794,16 @@
     </row>
     <row r="6">
       <c r="A6" s="204" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B6" s="204" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C6" s="198" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D6" s="204" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E6" s="205">
         <v>45602.0</v>
@@ -42716,7 +42824,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="206" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="M6" s="207"/>
       <c r="N6" s="208"/>
@@ -42735,13 +42843,13 @@
     </row>
     <row r="7">
       <c r="A7" s="181" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B7" s="190" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C7" s="209" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D7" s="203" t="s">
         <v>65</v>
@@ -42765,7 +42873,7 @@
       </c>
       <c r="K7" s="203"/>
       <c r="L7" s="211" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="M7" s="212"/>
       <c r="N7" s="212"/>
@@ -42784,14 +42892,14 @@
     </row>
     <row r="8">
       <c r="A8" s="213" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B8" s="214" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C8" s="215"/>
       <c r="D8" s="215" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E8" s="216">
         <v>45603.0</v>
@@ -42812,7 +42920,7 @@
       </c>
       <c r="K8" s="216"/>
       <c r="L8" s="218" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="M8" s="182"/>
       <c r="N8" s="182"/>
@@ -42831,16 +42939,16 @@
     </row>
     <row r="9">
       <c r="A9" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B9" s="220" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C9" s="221" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D9" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E9" s="223">
         <v>45671.0</v>
@@ -42849,7 +42957,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="221" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="H9" s="223">
         <v>45680.0</v>
@@ -42863,7 +42971,7 @@
       </c>
       <c r="K9" s="221"/>
       <c r="L9" s="225" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="M9" s="226"/>
       <c r="N9" s="226"/>
@@ -42882,14 +42990,14 @@
     </row>
     <row r="10">
       <c r="A10" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B10" s="227"/>
       <c r="C10" s="225" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D10" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E10" s="223">
         <v>45671.0</v>
@@ -42908,7 +43016,7 @@
       <c r="J10" s="221"/>
       <c r="K10" s="221"/>
       <c r="L10" s="225" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="M10" s="226"/>
       <c r="N10" s="226"/>
@@ -42927,14 +43035,14 @@
     </row>
     <row r="11">
       <c r="A11" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B11" s="227"/>
       <c r="C11" s="225" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D11" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E11" s="223">
         <v>45671.0</v>
@@ -42953,7 +43061,7 @@
       <c r="J11" s="221"/>
       <c r="K11" s="221"/>
       <c r="L11" s="225" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="M11" s="226"/>
       <c r="N11" s="226"/>
@@ -42972,14 +43080,14 @@
     </row>
     <row r="12">
       <c r="A12" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B12" s="227"/>
       <c r="C12" s="225" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D12" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E12" s="223">
         <v>45671.0</v>
@@ -42998,7 +43106,7 @@
       <c r="J12" s="221"/>
       <c r="K12" s="221"/>
       <c r="L12" s="225" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="M12" s="226"/>
       <c r="N12" s="226"/>
@@ -43017,14 +43125,14 @@
     </row>
     <row r="13">
       <c r="A13" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B13" s="227"/>
       <c r="C13" s="225" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D13" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E13" s="223">
         <v>45671.0</v>
@@ -43043,7 +43151,7 @@
       <c r="J13" s="221"/>
       <c r="K13" s="221"/>
       <c r="L13" s="225" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="M13" s="226"/>
       <c r="N13" s="226"/>
@@ -43062,14 +43170,14 @@
     </row>
     <row r="14">
       <c r="A14" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B14" s="227"/>
       <c r="C14" s="225" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="222" t="s">
         <v>190</v>
-      </c>
-      <c r="D14" s="222" t="s">
-        <v>182</v>
       </c>
       <c r="E14" s="223">
         <v>45671.0</v>
@@ -43088,7 +43196,7 @@
       <c r="J14" s="221"/>
       <c r="K14" s="221"/>
       <c r="L14" s="221" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="M14" s="226"/>
       <c r="N14" s="226"/>
@@ -43107,14 +43215,14 @@
     </row>
     <row r="15">
       <c r="A15" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B15" s="227"/>
       <c r="C15" s="225" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D15" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E15" s="223">
         <v>45671.0</v>
@@ -43133,7 +43241,7 @@
       <c r="J15" s="221"/>
       <c r="K15" s="221"/>
       <c r="L15" s="221" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="M15" s="226"/>
       <c r="N15" s="226"/>
@@ -43152,14 +43260,14 @@
     </row>
     <row r="16">
       <c r="A16" s="219" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B16" s="228"/>
       <c r="C16" s="229" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D16" s="222" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E16" s="223">
         <v>45681.0</v>
@@ -43178,7 +43286,7 @@
       <c r="J16" s="221"/>
       <c r="K16" s="221"/>
       <c r="L16" s="225" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="M16" s="226"/>
       <c r="N16" s="226"/>
@@ -49714,7 +49822,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="226" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49722,7 +49830,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="226" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49730,7 +49838,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="226" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49738,7 +49846,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="226" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49746,7 +49854,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="226" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49754,7 +49862,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="226" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49762,7 +49870,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="226" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49770,7 +49878,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="226" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49778,7 +49886,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="226" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49786,7 +49894,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="226" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49794,7 +49902,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="226" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49802,7 +49910,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="226" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49810,7 +49918,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="226" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49818,7 +49926,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="226" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49826,7 +49934,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="226" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49834,7 +49942,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="226" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49842,7 +49950,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="226" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49850,7 +49958,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="226" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50866,7 +50974,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="231" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B1" s="226"/>
       <c r="C1" s="226"/>
@@ -50924,7 +51032,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="232" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B3" s="233">
         <v>45596.0</v>
@@ -51217,261 +51325,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="236" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B4" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C4" s="238" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="J4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="L4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="M4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="N4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="O4" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P4" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="R4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="T4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="U4" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="V4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE4" s="241" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="AF4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL4" s="241" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="AM4" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AN4" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AO4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP4" s="241" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="AQ4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS4" s="241" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="AT4" s="242" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AV4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY4" s="241" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="AZ4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BA4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BH4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI4" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ4" s="241" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="BK4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BL4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BM4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BN4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BO4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BP4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BQ4" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BR4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CA4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CB4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CC4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CD4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG4" s="239"/>
       <c r="CH4" s="239"/>
       <c r="CI4" s="241" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="CJ4" s="239"/>
       <c r="CK4" s="239"/>
@@ -51483,249 +51591,249 @@
       <c r="CQ4" s="239"/>
       <c r="CR4" s="239"/>
       <c r="CS4" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="236" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B5" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="J5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="L5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="M5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="N5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="O5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="P5" s="240" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="Q5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="R5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="T5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="U5" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE5" s="243"/>
       <c r="AF5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL5" s="243"/>
       <c r="AM5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AN5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AO5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP5" s="243"/>
       <c r="AQ5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AR5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AS5" s="243"/>
       <c r="AT5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AU5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AV5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AW5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AX5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="AY5" s="243"/>
       <c r="AZ5" s="239" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="BA5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BH5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI5" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ5" s="243"/>
       <c r="BK5" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL5" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN5" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BP5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BQ5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BR5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CA5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CB5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CC5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CD5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG5" s="239"/>
       <c r="CH5" s="239"/>
@@ -51740,249 +51848,249 @@
       <c r="CQ5" s="239"/>
       <c r="CR5" s="239"/>
       <c r="CS5" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="236" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B6" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="J6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K6" s="244" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="M6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="N6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="O6" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P6" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="R6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="T6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="U6" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE6" s="243"/>
       <c r="AF6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL6" s="243"/>
       <c r="AM6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AN6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AO6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP6" s="243"/>
       <c r="AQ6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS6" s="243"/>
       <c r="AT6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AV6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY6" s="243"/>
       <c r="AZ6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BA6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BH6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI6" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ6" s="243"/>
       <c r="BK6" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL6" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM6" s="239" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="BN6" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BP6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BQ6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BR6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CA6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CB6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CC6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CD6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG6" s="239"/>
       <c r="CH6" s="239"/>
@@ -51997,198 +52105,198 @@
       <c r="CQ6" s="239"/>
       <c r="CR6" s="239"/>
       <c r="CS6" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="236" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="237" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="I7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="J7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="K7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="L7" s="244" t="s">
+        <v>232</v>
+      </c>
+      <c r="M7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="N7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="O7" s="239" t="s">
+        <v>225</v>
+      </c>
+      <c r="P7" s="240" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="R7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="S7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="T7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="U7" s="240" t="s">
+        <v>235</v>
+      </c>
+      <c r="V7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="W7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="X7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y7" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z7" s="239" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="237" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="D7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="E7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="F7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="H7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="I7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="J7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="K7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="L7" s="244" t="s">
-        <v>224</v>
-      </c>
-      <c r="M7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="N7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="O7" s="239" t="s">
-        <v>217</v>
-      </c>
-      <c r="P7" s="240" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="R7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="S7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="T7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="U7" s="240" t="s">
-        <v>227</v>
-      </c>
-      <c r="V7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="W7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="X7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="Y7" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z7" s="239" t="s">
-        <v>218</v>
-      </c>
       <c r="AA7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE7" s="243"/>
       <c r="AF7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL7" s="243"/>
       <c r="AM7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AN7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AO7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP7" s="243"/>
       <c r="AQ7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS7" s="243"/>
       <c r="AT7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU7" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AV7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY7" s="243"/>
       <c r="AZ7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BA7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BH7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI7" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ7" s="243"/>
       <c r="BK7" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL7" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN7" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO7" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BP7" s="239"/>
       <c r="BQ7" s="239"/>
@@ -52196,16 +52304,16 @@
       <c r="BS7" s="239"/>
       <c r="BT7" s="239"/>
       <c r="BU7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX7" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY7" s="239"/>
       <c r="BZ7" s="239"/>
@@ -52231,220 +52339,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="236" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B8" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="J8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="L8" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="M8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="N8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="O8" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P8" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="R8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="T8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="U8" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W8" s="239" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="X8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB8" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AC8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE8" s="243"/>
       <c r="AF8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL8" s="243"/>
       <c r="AM8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AN8" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AO8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP8" s="243"/>
       <c r="AQ8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS8" s="243"/>
       <c r="AT8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AV8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY8" s="243"/>
       <c r="AZ8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BA8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG8" s="239" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="BH8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI8" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ8" s="243"/>
       <c r="BK8" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL8" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN8" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BP8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BQ8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BR8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW8" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX8" s="239" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BY8" s="239"/>
       <c r="BZ8" s="239"/>
@@ -52470,244 +52578,244 @@
     </row>
     <row r="9">
       <c r="A9" s="236" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="237" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="G9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="H9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="I9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="J9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="K9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="L9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="M9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="N9" s="239" t="s">
+        <v>223</v>
+      </c>
+      <c r="O9" s="244" t="s">
         <v>232</v>
       </c>
-      <c r="B9" s="237" t="s">
-        <v>215</v>
-      </c>
-      <c r="C9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="D9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="E9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="F9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="G9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="H9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="I9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="J9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="K9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="L9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="M9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="N9" s="239" t="s">
-        <v>215</v>
-      </c>
-      <c r="O9" s="244" t="s">
-        <v>224</v>
-      </c>
       <c r="P9" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="R9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="T9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="U9" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE9" s="243"/>
       <c r="AF9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL9" s="243"/>
       <c r="AM9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AN9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AO9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP9" s="243"/>
       <c r="AQ9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS9" s="243"/>
       <c r="AT9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AV9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY9" s="243"/>
       <c r="AZ9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BA9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BH9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI9" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ9" s="243"/>
       <c r="BK9" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL9" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN9" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BP9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BQ9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BR9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CA9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CB9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CC9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CD9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG9" s="239"/>
       <c r="CH9" s="239"/>
@@ -52722,249 +52830,249 @@
       <c r="CQ9" s="239"/>
       <c r="CR9" s="239"/>
       <c r="CS9" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="236" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B10" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="J10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="L10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="M10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="N10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="O10" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P10" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="Q10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="R10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="T10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="U10" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="V10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AE10" s="243"/>
       <c r="AF10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AL10" s="243"/>
       <c r="AM10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AN10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AO10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP10" s="243"/>
       <c r="AQ10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS10" s="243"/>
       <c r="AT10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AV10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY10" s="243"/>
       <c r="AZ10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BA10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BB10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BC10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BD10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BE10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BF10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BG10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BH10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI10" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ10" s="243"/>
       <c r="BK10" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL10" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN10" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BP10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BQ10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BR10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW10" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BX10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CA10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CB10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CC10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CD10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG10" s="239"/>
       <c r="CH10" s="239"/>
@@ -52979,249 +53087,249 @@
       <c r="CQ10" s="239"/>
       <c r="CR10" s="239"/>
       <c r="CS10" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="236" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B11" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="J11" s="239" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="K11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="L11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="M11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="N11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="O11" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P11" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="R11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="S11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="T11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="U11" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="V11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Y11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Z11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AB11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AC11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AE11" s="243"/>
       <c r="AF11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AG11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AH11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AI11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL11" s="243"/>
       <c r="AM11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AN11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AO11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AP11" s="243"/>
       <c r="AQ11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AR11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AS11" s="243"/>
       <c r="AT11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AU11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AV11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AW11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AY11" s="243"/>
       <c r="AZ11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BA11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BB11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BC11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BE11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BF11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BG11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BH11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI11" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BJ11" s="243"/>
       <c r="BK11" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BL11" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BM11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN11" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BO11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BP11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BQ11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BR11" s="239" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="BS11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BT11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BU11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BX11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BY11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CA11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CB11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CC11" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CD11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG11" s="239"/>
       <c r="CH11" s="239"/>
@@ -53236,249 +53344,249 @@
       <c r="CQ11" s="239"/>
       <c r="CR11" s="239"/>
       <c r="CS11" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="236" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B12" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="G12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="H12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="J12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="L12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="M12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="N12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="O12" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P12" s="240" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="R12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="S12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="T12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="U12" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="V12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="W12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="X12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="Y12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="Z12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AA12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AB12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AC12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AE12" s="243"/>
       <c r="AF12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AG12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AH12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AI12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AJ12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AK12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AL12" s="243"/>
       <c r="AM12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AN12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AO12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AP12" s="243"/>
       <c r="AQ12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AR12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AS12" s="243"/>
       <c r="AT12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AU12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AV12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AW12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AX12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AY12" s="243"/>
       <c r="AZ12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BA12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BB12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BC12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BD12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BE12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BF12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BG12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BH12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BI12" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BJ12" s="243"/>
       <c r="BK12" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BL12" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BM12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BN12" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BO12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BP12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BQ12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BR12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BS12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BT12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BU12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BV12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BW12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BX12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BY12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="BZ12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CA12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CB12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CC12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CD12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CE12" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CG12" s="239"/>
       <c r="CH12" s="239"/>
@@ -53493,249 +53601,249 @@
       <c r="CQ12" s="239"/>
       <c r="CR12" s="239"/>
       <c r="CS12" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="236" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B13" s="237" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="F13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="G13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="H13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="I13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="J13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="K13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="L13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="M13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="N13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="O13" s="239" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="P13" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="Q13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="R13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="S13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="T13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="U13" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="V13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="W13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="X13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="Y13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="Z13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AA13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AB13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AC13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AD13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AE13" s="245"/>
       <c r="AF13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AG13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AH13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AI13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="AJ13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AK13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AL13" s="245"/>
       <c r="AM13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AN13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AO13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AP13" s="245"/>
       <c r="AQ13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AR13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AS13" s="245"/>
       <c r="AT13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AU13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AV13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AW13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AX13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AY13" s="245"/>
       <c r="AZ13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BA13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BB13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BC13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BD13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BE13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BF13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BG13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BH13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BI13" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BJ13" s="245"/>
       <c r="BK13" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BL13" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BM13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BN13" s="240" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BO13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BP13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BQ13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BR13" s="239" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="BS13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BT13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BU13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BV13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BW13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BX13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BY13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="BZ13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CA13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CB13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CC13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="CD13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CE13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CF13" s="239" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="CG13" s="239"/>
       <c r="CH13" s="239"/>
@@ -53750,7 +53858,7 @@
       <c r="CQ13" s="239"/>
       <c r="CR13" s="239"/>
       <c r="CS13" s="239" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54776,7 +54884,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="246" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B1" s="246" t="s">
         <v>2</v>
@@ -54803,13 +54911,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="250" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="K1" s="251" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="L1" s="249" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="M1" s="252"/>
       <c r="N1" s="252"/>
@@ -54828,10 +54936,10 @@
     </row>
     <row r="2">
       <c r="A2" s="253" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B2" s="254" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C2" s="255"/>
       <c r="D2" s="255" t="s">
@@ -54858,7 +54966,7 @@
       </c>
       <c r="K2" s="258"/>
       <c r="L2" s="259" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="M2" s="252"/>
       <c r="N2" s="252"/>
@@ -54877,16 +54985,16 @@
     </row>
     <row r="3">
       <c r="A3" s="253" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B3" s="260" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="C3" s="261" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D3" s="255" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E3" s="256">
         <v>45575.0</v>
@@ -54905,7 +55013,7 @@
       </c>
       <c r="K3" s="256"/>
       <c r="L3" s="259" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="M3" s="262"/>
       <c r="N3" s="252"/>
@@ -54924,14 +55032,14 @@
     </row>
     <row r="4">
       <c r="A4" s="253" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B4" s="243"/>
       <c r="C4" s="263" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="D4" s="255" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E4" s="256">
         <v>45575.0</v>
@@ -54950,7 +55058,7 @@
       </c>
       <c r="K4" s="264"/>
       <c r="L4" s="267" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="M4" s="262"/>
       <c r="N4" s="252"/>
@@ -54969,16 +55077,16 @@
     </row>
     <row r="5">
       <c r="A5" s="253" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B5" s="249" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="C5" s="255" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="D5" s="255" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E5" s="256">
         <v>45575.0</v>
@@ -54997,7 +55105,7 @@
       </c>
       <c r="K5" s="256"/>
       <c r="L5" s="259" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="M5" s="262"/>
       <c r="N5" s="252"/>

</xml_diff>